<commit_message>
final Day 30 CFU spleen
</commit_message>
<xml_diff>
--- a/SVX_Boost2X_Spleen_Day30_cfu_numbers.xlsx
+++ b/SVX_Boost2X_Spleen_Day30_cfu_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/rstor-henao_lab/Pablo/CFU_Pipeline/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1511A1FD-C92A-1845-92BC-F3B4C32E42F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DB6C24C-F79D-0F48-8C66-1B6A1F655EA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1280" yWindow="500" windowWidth="35840" windowHeight="21600" activeTab="1" xr2:uid="{F188F32F-936C-7746-94B2-81166A817508}"/>
+    <workbookView xWindow="14960" yWindow="500" windowWidth="35840" windowHeight="21600" activeTab="1" xr2:uid="{F188F32F-936C-7746-94B2-81166A817508}"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -615,7 +615,7 @@
   <dimension ref="A1:P131"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I39" sqref="I39"/>
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1557,7 +1557,9 @@
       <c r="J19" s="2">
         <v>13</v>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="2">
+        <v>0</v>
+      </c>
       <c r="L19" s="2">
         <v>0</v>
       </c>
@@ -1906,12 +1908,18 @@
       <c r="K26" s="2">
         <v>5</v>
       </c>
-      <c r="L26" s="2"/>
+      <c r="L26" s="2">
+        <v>0</v>
+      </c>
       <c r="M26" s="2">
         <v>1</v>
       </c>
-      <c r="N26" s="2"/>
-      <c r="O26" s="2"/>
+      <c r="N26" s="2">
+        <v>0</v>
+      </c>
+      <c r="O26" s="2">
+        <v>0</v>
+      </c>
       <c r="P26" s="2">
         <v>0</v>
       </c>
@@ -2450,10 +2458,18 @@
       <c r="K37" s="2">
         <v>0</v>
       </c>
-      <c r="L37" s="2"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="2"/>
-      <c r="O37" s="2"/>
+      <c r="L37" s="2">
+        <v>0</v>
+      </c>
+      <c r="M37" s="2">
+        <v>0</v>
+      </c>
+      <c r="N37" s="2">
+        <v>0</v>
+      </c>
+      <c r="O37" s="2">
+        <v>0</v>
+      </c>
       <c r="P37" s="2">
         <v>0</v>
       </c>

</xml_diff>